<commit_message>
Added more details from quest data
</commit_message>
<xml_diff>
--- a/DataCollection/QuestionnaireData/QuestionnaireScores.xlsx
+++ b/DataCollection/QuestionnaireData/QuestionnaireScores.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e005b3f8b47b9365/Documents/GitHub/KetamineProject/DataCollection/QuestionnaireData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\platon.uio.no\med-imb-u1\andrlm\pc\Dokumenter\GitHub\Ketamine-project\DataCollection\QuestionnaireData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1042" documentId="8_{B923416A-27A6-49F9-A36B-819DCEE54F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB300ACB-F0C4-425B-B55D-EBD13068A79E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{CF087212-1CDB-49D7-B2CC-BD48A3162A13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$C$206</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="240">
   <si>
     <t>Participant ID</t>
   </si>
@@ -750,12 +749,21 @@
   </si>
   <si>
     <t>SD5008</t>
+  </si>
+  <si>
+    <t>SD5009</t>
+  </si>
+  <si>
+    <t>Cannabis, lystgass</t>
+  </si>
+  <si>
+    <t>LSD, psilocybin, N-DMT, 25I-NBOME, 2C-B, 2C-B-FLY, ketamin, 3-MED-PCE, NXP, MXiPV, DPD, Ayahuasca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1148,39 +1156,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC866368-67E2-4042-AD5F-E3AC44C2CBE5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="J152" sqref="J152"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="10" max="10" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.7265625" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" customWidth="1"/>
-    <col min="24" max="24" width="20.54296875" customWidth="1"/>
-    <col min="25" max="25" width="15.81640625" customWidth="1"/>
-    <col min="26" max="26" width="20.81640625" customWidth="1"/>
-    <col min="27" max="27" width="21.81640625" customWidth="1"/>
-    <col min="28" max="28" width="24.26953125" customWidth="1"/>
-    <col min="29" max="29" width="23.7265625" customWidth="1"/>
-    <col min="30" max="30" width="19.26953125" customWidth="1"/>
-    <col min="31" max="31" width="17.81640625" customWidth="1"/>
-    <col min="32" max="32" width="18.26953125" customWidth="1"/>
-    <col min="33" max="33" width="12.7265625" customWidth="1"/>
-    <col min="34" max="34" width="17.54296875" customWidth="1"/>
-    <col min="35" max="35" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" customWidth="1"/>
+    <col min="26" max="26" width="20.85546875" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" customWidth="1"/>
+    <col min="28" max="28" width="24.28515625" customWidth="1"/>
+    <col min="29" max="29" width="23.7109375" customWidth="1"/>
+    <col min="30" max="30" width="19.28515625" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" customWidth="1"/>
+    <col min="32" max="32" width="18.28515625" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" customWidth="1"/>
+    <col min="34" max="34" width="17.5703125" customWidth="1"/>
+    <col min="35" max="35" width="18.28515625" customWidth="1"/>
     <col min="38" max="38" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1196,7 +1204,9 @@
       <c r="E1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>237</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1230,7 +1240,7 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1256,9 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1278,7 +1290,7 @@
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1294,7 +1306,9 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1308,7 +1322,7 @@
       <c r="Q3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1323,12 +1337,15 @@
       </c>
       <c r="E4" s="1">
         <v>27</v>
+      </c>
+      <c r="F4" s="1">
+        <v>32</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1343,12 +1360,15 @@
       </c>
       <c r="E5" s="1">
         <v>198</v>
+      </c>
+      <c r="F5" s="1">
+        <v>187</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1363,12 +1383,15 @@
       </c>
       <c r="E6" s="1">
         <v>90</v>
+      </c>
+      <c r="F6" s="1">
+        <v>78</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1382,13 +1405,16 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1402,13 +1428,16 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
         <v>0</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1422,13 +1451,16 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>218</v>
       </c>
@@ -1443,12 +1475,15 @@
       </c>
       <c r="E10" s="1">
         <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1460,11 +1495,14 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>219</v>
       </c>
@@ -1478,13 +1516,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1499,12 +1540,15 @@
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1518,13 +1562,16 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1538,13 +1585,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
         <v>0</v>
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1558,13 +1608,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1578,13 +1631,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -1599,12 +1655,15 @@
       </c>
       <c r="E18" s="1">
         <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="W18" s="1"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -1618,13 +1677,16 @@
         <v>1</v>
       </c>
       <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="W19" s="1"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -1638,13 +1700,16 @@
         <v>1</v>
       </c>
       <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="W20" s="1"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>235</v>
       </c>
@@ -1664,11 +1729,15 @@
         <f>AVERAGE(E16:E20)</f>
         <v>1.2</v>
       </c>
+      <c r="F21" s="1">
+        <f>AVERAGE(F16:F20)</f>
+        <v>1</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1682,13 +1751,16 @@
         <v>1</v>
       </c>
       <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="W22" s="1"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
@@ -1703,12 +1775,15 @@
       </c>
       <c r="E23" s="1">
         <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="W23" s="1"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1724,8 +1799,11 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -1741,8 +1819,11 @@
       <c r="E25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -1758,8 +1839,11 @@
       <c r="E26" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>220</v>
       </c>
@@ -1776,10 +1860,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E27:M27" si="0">AVERAGE(E16:E26)</f>
+        <f t="shared" ref="E27:F27" si="0">AVERAGE(E16:E26)</f>
         <v>1.3818181818181818</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1788,7 +1875,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
@@ -1804,8 +1891,11 @@
       <c r="E28" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F28" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
@@ -1821,8 +1911,11 @@
       <c r="E29" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F29" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>32</v>
       </c>
@@ -1838,8 +1931,11 @@
       <c r="E30" s="1">
         <v>32.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F30" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -1859,8 +1955,12 @@
         <f>AVERAGE(E28:E30)</f>
         <v>56.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F31" s="1">
+        <f>AVERAGE(F28:F30)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1876,8 +1976,11 @@
       <c r="E32" s="1">
         <v>32.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
@@ -1893,8 +1996,11 @@
       <c r="E33" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F33" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -1910,8 +2016,11 @@
       <c r="E34" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F34" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>200</v>
       </c>
@@ -1927,8 +2036,11 @@
       <c r="E35" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>201</v>
       </c>
@@ -1944,8 +2056,11 @@
       <c r="E36" s="1">
         <v>87.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F36" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>202</v>
       </c>
@@ -1961,8 +2076,11 @@
       <c r="E37" s="1">
         <v>87.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F37" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>203</v>
       </c>
@@ -1978,8 +2096,11 @@
       <c r="E38" s="1">
         <v>62.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F38" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>204</v>
       </c>
@@ -1995,8 +2116,11 @@
       <c r="E39" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F39" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>205</v>
       </c>
@@ -2012,8 +2136,11 @@
       <c r="E40" s="1">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F40" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>222</v>
       </c>
@@ -2033,8 +2160,12 @@
         <f>AVERAGE(E32:E40)</f>
         <v>59.166666666666664</v>
       </c>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <f>AVERAGE(F32:F40)</f>
+        <v>63.888888888888886</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
@@ -2050,8 +2181,11 @@
       <c r="E42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>18</v>
       </c>
@@ -2067,7 +2201,9 @@
       <c r="E43" s="1">
         <v>0</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -2101,7 +2237,7 @@
       <c r="AK43" s="1"/>
       <c r="AL43" s="1"/>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>19</v>
       </c>
@@ -2117,7 +2253,9 @@
       <c r="E44" s="1">
         <v>1</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2149,7 +2287,7 @@
       <c r="AK44" s="1"/>
       <c r="AL44" s="1"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>20</v>
       </c>
@@ -2165,7 +2303,9 @@
       <c r="E45" s="1">
         <v>0</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2179,7 +2319,7 @@
       <c r="Q45" s="1"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>21</v>
       </c>
@@ -2195,8 +2335,11 @@
       <c r="E46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>22</v>
       </c>
@@ -2212,8 +2355,11 @@
       <c r="E47" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>23</v>
       </c>
@@ -2229,8 +2375,11 @@
       <c r="E48" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>24</v>
       </c>
@@ -2246,8 +2395,11 @@
       <c r="E49" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
@@ -2263,8 +2415,11 @@
       <c r="E50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>223</v>
       </c>
@@ -2284,8 +2439,12 @@
         <f>AVERAGE(E42:E50)</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51">
+        <f>AVERAGE(F42:F50)</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>42</v>
       </c>
@@ -2301,8 +2460,11 @@
       <c r="E52" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>43</v>
       </c>
@@ -2318,8 +2480,11 @@
       <c r="E53" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>44</v>
       </c>
@@ -2335,8 +2500,11 @@
       <c r="E54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>61</v>
       </c>
@@ -2352,8 +2520,11 @@
       <c r="E55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>45</v>
       </c>
@@ -2369,8 +2540,11 @@
       <c r="E56" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -2386,8 +2560,11 @@
       <c r="E57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -2403,8 +2580,11 @@
       <c r="E58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2420,8 +2600,11 @@
       <c r="E59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -2437,8 +2620,11 @@
       <c r="E60" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -2454,8 +2640,11 @@
       <c r="E61" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -2471,8 +2660,11 @@
       <c r="E62" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -2488,8 +2680,11 @@
       <c r="E63" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -2505,8 +2700,11 @@
       <c r="E64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>54</v>
       </c>
@@ -2522,8 +2720,11 @@
       <c r="E65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -2539,8 +2740,11 @@
       <c r="E66" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -2556,8 +2760,11 @@
       <c r="E67" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -2573,8 +2780,11 @@
       <c r="E68" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -2590,8 +2800,11 @@
       <c r="E69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -2607,8 +2820,11 @@
       <c r="E70" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -2624,8 +2840,11 @@
       <c r="E71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>224</v>
       </c>
@@ -2645,8 +2864,12 @@
         <f>AVERAGE(E52,E54,E56,E60,E61,E63,E65,E67,E68,E70)</f>
         <v>1.4</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72" s="1">
+        <f>AVERAGE(F52,F54,F56,F60,F61,F63,F65,F67,F68,F70)</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>225</v>
       </c>
@@ -2666,8 +2889,12 @@
         <f>AVERAGE(E53,E55,E57,E58,E59,E62,E64,E66,E69,E71)</f>
         <v>0.7</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73" s="1">
+        <f>AVERAGE(F53,F55,F57,F58,F59,F62,F64,F66,F69,F71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>62</v>
       </c>
@@ -2683,8 +2910,11 @@
       <c r="E74" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -2700,8 +2930,11 @@
       <c r="E75" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>64</v>
       </c>
@@ -2717,8 +2950,11 @@
       <c r="E76" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>65</v>
       </c>
@@ -2734,8 +2970,11 @@
       <c r="E77" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -2751,8 +2990,11 @@
       <c r="E78" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -2768,8 +3010,11 @@
       <c r="E79" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -2785,8 +3030,11 @@
       <c r="E80" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>69</v>
       </c>
@@ -2802,8 +3050,11 @@
       <c r="E81" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>70</v>
       </c>
@@ -2819,8 +3070,11 @@
       <c r="E82" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>71</v>
       </c>
@@ -2836,8 +3090,11 @@
       <c r="E83" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>226</v>
       </c>
@@ -2857,8 +3114,12 @@
         <f>AVERAGE(E74:E83)</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" s="1">
+        <f>AVERAGE(F74:F83)</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>72</v>
       </c>
@@ -2869,7 +3130,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -2880,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>75</v>
       </c>
@@ -2891,13 +3152,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>74</v>
       </c>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -2908,7 +3169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -2919,7 +3180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -2930,7 +3191,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>84</v>
       </c>
@@ -2941,7 +3202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>79</v>
       </c>
@@ -2950,14 +3211,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>80</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>81</v>
       </c>
@@ -2968,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>82</v>
       </c>
@@ -2979,7 +3240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -2990,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -3001,7 +3262,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>86</v>
       </c>
@@ -3012,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -3023,14 +3284,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>88</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -3041,7 +3302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>90</v>
       </c>
@@ -3052,7 +3313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -3063,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>91</v>
       </c>
@@ -3074,7 +3335,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>92</v>
       </c>
@@ -3085,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>93</v>
       </c>
@@ -3096,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>94</v>
       </c>
@@ -3104,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>95</v>
       </c>
@@ -3115,7 +3376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>96</v>
       </c>
@@ -3126,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -3137,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -3148,7 +3409,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>98</v>
       </c>
@@ -3159,7 +3420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>99</v>
       </c>
@@ -3170,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>100</v>
       </c>
@@ -3178,7 +3439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -3189,7 +3450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>102</v>
       </c>
@@ -3200,7 +3461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>109</v>
       </c>
@@ -3211,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>111</v>
       </c>
@@ -3222,7 +3483,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>113</v>
       </c>
@@ -3233,7 +3494,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>115</v>
       </c>
@@ -3244,7 +3505,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -3255,7 +3516,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -3266,7 +3527,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -3277,7 +3538,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -3289,7 +3550,7 @@
       </c>
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -3305,8 +3566,11 @@
       <c r="E126" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F126" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -3322,8 +3586,11 @@
       <c r="E127" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F127" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -3339,8 +3606,11 @@
       <c r="E128" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F128" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -3356,8 +3626,11 @@
       <c r="E129" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F129" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -3373,8 +3646,11 @@
       <c r="E130" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F130" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -3390,8 +3666,11 @@
       <c r="E131" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F131" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>227</v>
       </c>
@@ -3411,8 +3690,12 @@
         <f>AVERAGE(E126:E131)</f>
         <v>17.666666666666668</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F132" s="1">
+        <f>AVERAGE(F126:F131)</f>
+        <v>56.666666666666664</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -3428,8 +3711,11 @@
       <c r="E133" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F133" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -3445,8 +3731,11 @@
       <c r="E134" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F134" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -3462,8 +3751,11 @@
       <c r="E135" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F135" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -3479,8 +3771,11 @@
       <c r="E136" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F136" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -3496,8 +3791,11 @@
       <c r="E137" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F137" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>135</v>
       </c>
@@ -3513,8 +3811,11 @@
       <c r="E138" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F138" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -3530,8 +3831,11 @@
       <c r="E139" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F139" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>137</v>
       </c>
@@ -3547,8 +3851,11 @@
       <c r="E140" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F140" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>228</v>
       </c>
@@ -3568,8 +3875,12 @@
         <f>AVERAGE(E133,E137,E139,E140)</f>
         <v>66.25</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F141" s="1">
+        <f>AVERAGE(F133,F137,F139,F140)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>229</v>
       </c>
@@ -3589,8 +3900,12 @@
         <f>AVERAGE(E134,E135,E136,E138)</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F142" s="1">
+        <f>AVERAGE(F134,F135,F136,F138)</f>
+        <v>92.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -3606,8 +3921,11 @@
       <c r="E143" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>139</v>
       </c>
@@ -3623,8 +3941,11 @@
       <c r="E144" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F144" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -3640,8 +3961,11 @@
       <c r="E145" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F145" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>141</v>
       </c>
@@ -3657,8 +3981,11 @@
       <c r="E146" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>142</v>
       </c>
@@ -3674,8 +4001,11 @@
       <c r="E147" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>143</v>
       </c>
@@ -3691,8 +4021,11 @@
       <c r="E148" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F148" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>230</v>
       </c>
@@ -3710,8 +4043,11 @@
       <c r="E149" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F149" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>144</v>
       </c>
@@ -3728,7 +4064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -3745,7 +4081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>146</v>
       </c>
@@ -3762,7 +4098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>147</v>
       </c>
@@ -3779,7 +4115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>148</v>
       </c>
@@ -3796,7 +4132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>149</v>
       </c>
@@ -3813,7 +4149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>150</v>
       </c>
@@ -3830,7 +4166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>151</v>
       </c>
@@ -3847,7 +4183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3864,7 +4200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>153</v>
       </c>
@@ -3881,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>154</v>
       </c>
@@ -3898,7 +4234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>155</v>
       </c>
@@ -3915,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -3932,7 +4268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>156</v>
       </c>
@@ -3949,7 +4285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>157</v>
       </c>
@@ -3966,7 +4302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>158</v>
       </c>
@@ -3983,7 +4319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>159</v>
       </c>
@@ -4000,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>161</v>
       </c>
@@ -4017,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>162</v>
       </c>
@@ -4034,7 +4370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>206</v>
       </c>
@@ -4051,7 +4387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>163</v>
       </c>
@@ -4068,7 +4404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>164</v>
       </c>
@@ -4085,7 +4421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>165</v>
       </c>
@@ -4102,7 +4438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>166</v>
       </c>
@@ -4119,7 +4455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>167</v>
       </c>
@@ -4136,7 +4472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>231</v>
       </c>
@@ -4157,7 +4493,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>168</v>
       </c>
@@ -4174,7 +4510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>169</v>
       </c>
@@ -4191,7 +4527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>170</v>
       </c>
@@ -4208,7 +4544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>171</v>
       </c>
@@ -4225,7 +4561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>172</v>
       </c>
@@ -4242,7 +4578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>173</v>
       </c>
@@ -4259,7 +4595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>174</v>
       </c>
@@ -4276,7 +4612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>175</v>
       </c>
@@ -4293,7 +4629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>176</v>
       </c>
@@ -4310,7 +4646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>177</v>
       </c>
@@ -4327,7 +4663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>178</v>
       </c>
@@ -4344,7 +4680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>197</v>
       </c>
@@ -4361,7 +4697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>179</v>
       </c>
@@ -4378,7 +4714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>180</v>
       </c>
@@ -4395,7 +4731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>181</v>
       </c>
@@ -4412,7 +4748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>182</v>
       </c>
@@ -4429,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>183</v>
       </c>
@@ -4446,7 +4782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>184</v>
       </c>
@@ -4463,7 +4799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>185</v>
       </c>
@@ -4480,7 +4816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>186</v>
       </c>
@@ -4497,7 +4833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>187</v>
       </c>
@@ -4514,7 +4850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>188</v>
       </c>
@@ -4531,7 +4867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>189</v>
       </c>
@@ -4548,7 +4884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>190</v>
       </c>
@@ -4565,7 +4901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>191</v>
       </c>
@@ -4582,7 +4918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>192</v>
       </c>
@@ -4599,7 +4935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>193</v>
       </c>
@@ -4616,7 +4952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>194</v>
       </c>
@@ -4633,7 +4969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>195</v>
       </c>
@@ -4650,7 +4986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>196</v>
       </c>
@@ -4667,7 +5003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>232</v>
       </c>
@@ -4688,20 +5024,20 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C206" xr:uid="{FC866368-67E2-4042-AD5F-E3AC44C2CBE5}"/>
+  <autoFilter ref="A1:C206"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more participant data
</commit_message>
<xml_diff>
--- a/DataCollection/QuestionnaireData/QuestionnaireScores.xlsx
+++ b/DataCollection/QuestionnaireData/QuestionnaireScores.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="288">
   <si>
     <t>Participant ID</t>
   </si>
@@ -758,12 +758,159 @@
   </si>
   <si>
     <t>LSD, psilocybin, N-DMT, 25I-NBOME, 2C-B, 2C-B-FLY, ketamin, 3-MED-PCE, NXP, MXiPV, DPD, Ayahuasca</t>
+  </si>
+  <si>
+    <t>At jeg tenkte litt å hvordan det føles når jeg liggger her med hode. Vandret med tankene.</t>
+  </si>
+  <si>
+    <t>ouff ja, ehm vanskelig å forklare men ehm jeg opplevde at jeg reiste (?)</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Ehh hmm. Eehhm. Mye rart. Eeh jeg opplevde at jeg drømte at jeg tok en slags t-bane.</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ehh uhmm. kremt. Jeg opplevde at jeg </t>
+  </si>
+  <si>
+    <t>Ja hehe. Ja det var helt crazy. Det er vanskelig å forklare det også. Det var som om jeg ble transportert i en slags t-bane aktig verden. Noe mer? Jeg vet ikke. Det var veldig mye. Veldig mye lilla basically. Ehm jo det var jo ganske mye, jeg har sikkert glemt en del. Føltes ut som jeg ble smeltet. At jeg ble smeltet fast i det jeg ligger på og på en måte sendt langt bortover.</t>
+  </si>
+  <si>
+    <t>Ehh ja. Tenker du på eksperimentet? Ja, jeg vil påstå at jeg husker det meste av ekseperimentet før vi kom hit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, jeg hadde liksom flere. Ehh ja denen var at jeg ble smeltet inn i veggen bakken ogbevegde meg bortover. Ehm ehm kan egentlig ikke huske noen andre drømmer. </t>
+  </si>
+  <si>
+    <t>Det er jo at jeg lå her og fikk et stikk i armen. Etter det så ble jeg beruset. Husker du at du telte? JA Husker du hva du telte til? tror ejg kom til 120, 111 rundt der</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nei, det var veldig spenennde hihi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, men jeg husker ikke hva den heter. Ikke sikkert riktig, men jeg synes det luktet som grønn gugge på pizza. Fire lukter, si hvilken det var: JEg vet ikke ass, kanskje sour crout. </t>
+  </si>
+  <si>
+    <t>Ingenting, litt, noen bilder</t>
+  </si>
+  <si>
+    <t>Jeg opplevde å være manmge forskjellige bosteder og forflytte meg i tid og rom.</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>Jeg opplevde at jeg stod og snakket med noen - vet ikke hvem ,alt endrer seg hele tiden. </t>
+  </si>
+  <si>
+    <t>Umulig å si</t>
+  </si>
+  <si>
+    <t>Vet ikke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">språk er rart, betryggende å være her enn i hodet, genser er klumpete, alt føles så sykt oppblåst, [motorkontroll sånn passe], [hvor har du vært hen?] jeg har vært et sted som har vært mot domus på psi, kjente mye greier som jeg ikke kjønner noen ting av, [husker du hva som skjedde?] jeg husker det var ingenting som skjedde, bare ting skjedde, litt ut som å være fanget [[[k-hole?]]], litt som å ikke vite hvor ting er, [mistet du følelse av hvor du selv var`?] nei, … nå er vi her ja, [hvordan føles det?] føles rart, vært gjennom noe viktig, [14.12], det var veldig upersonlig, handlet ikke om noen ting, var bare strukturer og mønstre som passet sammen og bevegde seg, veldig rart, skjønner ikke hvor jeg er nå heller, [husker at vi kjørte ut hit], det var fint å ha deg nær, [tilstede i rommet her?] mer og mer som jeg er tilstede, stoppet dere forde jeg sa stopp? hvor lenge var jeg nede? [husker du hvorfor d ville stoppe?] veldig sterke opplevelse av å være et sted og møtte mennesker men alt var i sånn matriser, systematisk og riktig, følte veldig fanget, men ting gikk opp og rundt hverandre, ikke statisk, føltes som jeg var på spesifikke lokasjen, at jeg fysisk var der, virkeligheten ga ikke meniing, skjønte ikke hva som foregikk,da det ble skummelt, at jeg ble fastlåst i den form for virkelighet, det var veldig detaljrikt, når man er inni det så er det så ekte. Stemte ikke, denne virkeligheten og den inni der. Husker at jeg spurte om hva som skjedde. Føler at det hjalp å ha kontakt. HVis jeg var alene inni matriseverden så hadde det vært ubehagelig, kanskje. [14.22] konsepter sluttet å gi mening, føltes osm jeg skulle prestere ett eller annet, </t>
+  </si>
+  <si>
+    <t> ja husker du spurte om diverse byer og noen ord, og at jeg begynte å svare før du hadde sagt alle ordene,</t>
+  </si>
+  <si>
+    <t>jeg husker alt veldig klart og tydelig som om jeg var der, jeg opplevde å bli flyttet fra sted til sted, over tid, basert på at jeg visste at jeg var på eksperiment, men skjønte ikke helt hva som foregikk, husker at jeg spurte om det, husker å stå oppe ved domus der vi kjørte fra, teksturen og snøen var lik, sto på snøen, var i det, men alt var firkanter, og amtriser. Kunne bytte en virkelighet med en annen, noen steder var det hvitt og kaldt, noen steder blått, rødt og folk, grått, føltes som jeg var i sykehusgang. Men ble forflyttet, kontinuerlig.Noe flyttet emg, ble dratt rundt.</t>
+  </si>
+  <si>
+    <t>telle opp til 100, tror jeg kom til 140 ett eller annet</t>
+  </si>
+  <si>
+    <t>Nei</t>
+  </si>
+  <si>
+    <t>open choice: mener at jeg luktet persille hver eneste gang, 4choice: sauerkraut, 2fc: den første, (hvitløk)</t>
+  </si>
+  <si>
+    <t>jeg så den mørke fargen av lukke øye, behagelig følelse i kroppen, nesten som kroppen begynte å forsvinne litt. Avslappet emosjonelt. Litt søvnig. En slags dagdrøm</t>
+  </si>
+  <si>
+    <t>hva jeg opplevde`? jeg er usikker på om det er noen på forskjell mellom jeg og alt,</t>
+  </si>
+  <si>
+    <t>[en] religiøs opplevelse</t>
+  </si>
+  <si>
+    <t>jeg har et meta bevissthetsperspektiv jeg prøver å forstå mellom sammenhengen mellom jeg og annet</t>
+  </si>
+  <si>
+    <t>jeg kan prøve, jeg har definitivt opplevd i en endrin i perspektiv, sammenligne tmed normal bevissthetstilstand, - veldig mye å ta tak i, jeg vil første bemerke er at det har vært temaer gjennomgående i opplevelsen, som omhandler selvet, tid, rom, materie, relasjon mellom dem, selv og andre, under hele opplevelsen har jeg hatt en .. innhold hele veien - ikke på noe tidspunkt har det vært uten innhold, men innholdet er veldig annerledes enn det daglige, jeg har hatt en fornemmelse av å ha en kropp men grensen mellom kropp og omgivelsene syns å være noe utvisket. Opplevelsen av kroppen hvor stor de ulike delene er relativt til hverandre er forvrengt, vanskelig å sette tydelige grenser hvor.. smelter sammen eller glir over i hverandre. Føles som tiden går veldig sakte. Hvert øyeblikk varer veldig lenge, at det er mye rom for å undersøke hvert øyeblikk.Hele tiden en følelse av årvåkenhet - at jeg får med meg det som skjer. men ikke å være bevisstløs eller i dyp søvn.</t>
+  </si>
+  <si>
+    <t>hmm, jeg tenkte på at jeg syns at støtten som hodet mitt ligger på er litt ubehagelig, temperaturen kjennes fin, vært veldig stille, lite forstyrrelser, kunne undersøke egen bevissthet uten ekstern påvirkning</t>
+  </si>
+  <si>
+    <t>ja, det er vanskelig å huske det som skjedde lenger tilbake i tid, men relativt nylig - blant annet jeg er praktiserende buddhist der man visualeserer en guddom (tara), og tara dukket opp i bevisstheten min som det spontant dukket opp et mantra. Denne det at jeg så tara var assosiert med trygghet og kjærlighet, og takknemmelighet</t>
+  </si>
+  <si>
+    <t>at jeg telte oppover, [hvilke tall] - over 100, kan det ha vært 130 140 kanskje?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">det er veldig vanskelig å vurdere hvor lang tid som har gått - jeg har følt meg veldig trygg - </t>
+  </si>
+  <si>
+    <t>(husker at ble presentert for lukter) husker ikke hva men husker jeg sa sjokolade og plastelina, men vet ikke nå hva jeg luktet, (open choice): kakao? - 4ch: gulrot - 2ch: de var ikke helt like, men ganske like, jeg tror den siste (hvitløk)</t>
+  </si>
+  <si>
+    <t>SD5010</t>
+  </si>
+  <si>
+    <t>Alkohol</t>
+  </si>
+  <si>
+    <t>Ingenting</t>
+  </si>
+  <si>
+    <t>Aner ikke</t>
+  </si>
+  <si>
+    <t>masse, for mye (å beskrive)</t>
+  </si>
+  <si>
+    <t>godt spørsmål, (husker du?) nei</t>
+  </si>
+  <si>
+    <t>brah, husker ikke når det starta, telte til 60, så bare smelta verden eller noe sånt, også visste jeg ikke helt om jeg var drugget ned eller ikke, skjønte ikke hvem jeg var, hvor jeg var, så skjønte jeg hvor jeg var og hvem jeg var, at jeg var noe hvertfal - så var det masse shit som skjedde, husker jeg ikke så mye av. Hadde litt kontroll over hva jeg ville opplevele, til en hvis grad. Husker ikke helt hva jeg ville oppleve.. zoome gjennom verdensrommet. Husker ikke om jeg fikk oppleve det.</t>
+  </si>
+  <si>
+    <t>at du spurte meg liksom? husker at du spurte meg, at jeg ikke klarte å svare. Du spurte om land eller byer eller hovedstader, ord, de orda husker jeg ikke en shit av</t>
+  </si>
+  <si>
+    <t>ikke noe konkret</t>
+  </si>
+  <si>
+    <t>at jeg telte, 60 kom jeg til.</t>
+  </si>
+  <si>
+    <t>det var sykt, what the hell, var sånn.. tror ikke jeg skjønte når det kicket inn, har eksperimentet startet tenkte jeg, men var kanskje langt inni drømmeland. Hvorfor er jeg tenkte jeg</t>
+  </si>
+  <si>
+    <t>ja hva faen var det.. no idea, no oljete, 4ch: hvitløk. 2ch [eksperimentator ga svaret fra før] - den første - lett. (hvitløk)</t>
+  </si>
+  <si>
+    <t>Pilot_2001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -819,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,6 +985,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="I149" sqref="I149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,8 +1361,12 @@
       <c r="F1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1259,8 +1417,12 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1309,8 +1471,12 @@
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1341,6 +1507,12 @@
       <c r="F4" s="1">
         <v>32</v>
       </c>
+      <c r="G4" s="1">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1">
+        <v>23</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="W4" s="1"/>
@@ -1364,6 +1536,12 @@
       <c r="F5" s="1">
         <v>187</v>
       </c>
+      <c r="G5" s="1">
+        <v>192</v>
+      </c>
+      <c r="H5" s="1">
+        <v>185</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="W5" s="1"/>
@@ -1387,6 +1565,12 @@
       <c r="F6" s="1">
         <v>78</v>
       </c>
+      <c r="G6" s="1">
+        <v>106</v>
+      </c>
+      <c r="H6" s="1">
+        <v>75</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="W6" s="1"/>
@@ -1410,6 +1594,12 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="W7" s="1"/>
@@ -1433,6 +1623,12 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="W8" s="1"/>
@@ -1456,6 +1652,12 @@
       <c r="F9" s="1">
         <v>0</v>
       </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="W9" s="1"/>
@@ -1479,6 +1681,9 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="W10" s="1"/>
@@ -1487,16 +1692,19 @@
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>198</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>238</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1521,6 +1729,9 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="W12" s="1"/>
@@ -1544,6 +1755,9 @@
       <c r="F13" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="W13" s="1"/>
@@ -1567,6 +1781,9 @@
       <c r="F14" s="1">
         <v>0</v>
       </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="W14" s="1"/>
@@ -1590,6 +1807,9 @@
       <c r="F15" s="1">
         <v>0</v>
       </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="W15" s="1"/>
@@ -1613,6 +1833,9 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="W16" s="1"/>
@@ -1636,6 +1859,9 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="W17" s="1"/>
@@ -1659,6 +1885,9 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
+      <c r="G18" s="1">
+        <v>3</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="W18" s="1"/>
@@ -1682,6 +1911,9 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="W19" s="1"/>
@@ -1705,6 +1937,9 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="W20" s="1"/>
@@ -1733,6 +1968,10 @@
         <f>AVERAGE(F16:F20)</f>
         <v>1</v>
       </c>
+      <c r="G21" s="1">
+        <f>AVERAGE(G16:G20)</f>
+        <v>1.8</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="W21" s="1"/>
@@ -1756,6 +1995,9 @@
       <c r="F22" s="1">
         <v>1</v>
       </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="W22" s="1"/>
@@ -1779,6 +2021,9 @@
       <c r="F23" s="1">
         <v>1</v>
       </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="W23" s="1"/>
@@ -1802,6 +2047,9 @@
       <c r="F24" s="1">
         <v>1</v>
       </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1822,6 +2070,9 @@
       <c r="F25" s="1">
         <v>1</v>
       </c>
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -1842,6 +2093,9 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -1860,14 +2114,17 @@
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E27:F27" si="0">AVERAGE(E16:E26)</f>
+        <f t="shared" ref="E27:G27" si="0">AVERAGE(E16:E26)</f>
         <v>1.3818181818181818</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8909090909090909</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1894,6 +2151,9 @@
       <c r="F28" s="1">
         <v>100</v>
       </c>
+      <c r="G28" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -1914,6 +2174,9 @@
       <c r="F29" s="1">
         <v>100</v>
       </c>
+      <c r="G29" s="1">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -1934,6 +2197,9 @@
       <c r="F30" s="1">
         <v>100</v>
       </c>
+      <c r="G30" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1959,6 +2225,10 @@
         <f>AVERAGE(F28:F30)</f>
         <v>100</v>
       </c>
+      <c r="G31" s="1">
+        <f>AVERAGE(G28:G30)</f>
+        <v>61.666666666666664</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -1979,6 +2249,9 @@
       <c r="F32" s="1">
         <v>0</v>
       </c>
+      <c r="G32" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -1999,6 +2272,9 @@
       <c r="F33" s="1">
         <v>100</v>
       </c>
+      <c r="G33" s="1">
+        <v>90</v>
+      </c>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -2019,6 +2295,9 @@
       <c r="F34" s="1">
         <v>100</v>
       </c>
+      <c r="G34" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -2039,6 +2318,9 @@
       <c r="F35" s="1">
         <v>0</v>
       </c>
+      <c r="G35" s="1">
+        <v>65</v>
+      </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -2059,6 +2341,9 @@
       <c r="F36" s="1">
         <v>100</v>
       </c>
+      <c r="G36" s="1">
+        <v>75</v>
+      </c>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -2079,6 +2364,9 @@
       <c r="F37" s="1">
         <v>100</v>
       </c>
+      <c r="G37" s="1">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
@@ -2099,6 +2387,9 @@
       <c r="F38" s="1">
         <v>100</v>
       </c>
+      <c r="G38" s="1">
+        <v>95</v>
+      </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -2119,6 +2410,9 @@
       <c r="F39" s="1">
         <v>25</v>
       </c>
+      <c r="G39" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
@@ -2139,6 +2433,9 @@
       <c r="F40" s="1">
         <v>50</v>
       </c>
+      <c r="G40" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -2164,6 +2461,10 @@
         <f>AVERAGE(F32:F40)</f>
         <v>63.888888888888886</v>
       </c>
+      <c r="G41">
+        <f>AVERAGE(G32:G40)</f>
+        <v>67.777777777777771</v>
+      </c>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -2184,6 +2485,9 @@
       <c r="F42" s="1">
         <v>0</v>
       </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -2204,7 +2508,9 @@
       <c r="F43" s="1">
         <v>0</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1">
+        <v>4</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2256,7 +2562,9 @@
       <c r="F44" s="1">
         <v>1</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1">
+        <v>2</v>
+      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2306,7 +2614,9 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2338,6 +2648,9 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
+      <c r="G46" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
@@ -2358,6 +2671,9 @@
       <c r="F47" s="1">
         <v>0</v>
       </c>
+      <c r="G47" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -2378,8 +2694,11 @@
       <c r="F48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>24</v>
       </c>
@@ -2398,8 +2717,11 @@
       <c r="F49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
@@ -2418,8 +2740,11 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>223</v>
       </c>
@@ -2443,8 +2768,12 @@
         <f>AVERAGE(F42:F50)</f>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f>AVERAGE(G42:G50)</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>42</v>
       </c>
@@ -2463,8 +2792,11 @@
       <c r="F52" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>43</v>
       </c>
@@ -2483,8 +2815,11 @@
       <c r="F53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>44</v>
       </c>
@@ -2503,8 +2838,11 @@
       <c r="F54" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>61</v>
       </c>
@@ -2523,8 +2861,11 @@
       <c r="F55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>45</v>
       </c>
@@ -2543,8 +2884,11 @@
       <c r="F56" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -2563,8 +2907,11 @@
       <c r="F57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -2583,8 +2930,11 @@
       <c r="F58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2603,8 +2953,11 @@
       <c r="F59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -2623,8 +2976,11 @@
       <c r="F60" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -2643,8 +2999,11 @@
       <c r="F61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -2663,8 +3022,11 @@
       <c r="F62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -2683,8 +3045,11 @@
       <c r="F63" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -2703,8 +3068,11 @@
       <c r="F64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>54</v>
       </c>
@@ -2723,8 +3091,11 @@
       <c r="F65" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -2743,8 +3114,11 @@
       <c r="F66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -2763,8 +3137,11 @@
       <c r="F67" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -2783,8 +3160,11 @@
       <c r="F68" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -2803,8 +3183,11 @@
       <c r="F69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -2823,8 +3206,11 @@
       <c r="F70" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -2843,8 +3229,11 @@
       <c r="F71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>224</v>
       </c>
@@ -2868,8 +3257,12 @@
         <f>AVERAGE(F52,F54,F56,F60,F61,F63,F65,F67,F68,F70)</f>
         <v>2.8</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="1">
+        <f>AVERAGE(G52,G54,G56,G60,G61,G63,G65,G67,G68,G70)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>225</v>
       </c>
@@ -2893,8 +3286,12 @@
         <f>AVERAGE(F53,F55,F57,F58,F59,F62,F64,F66,F69,F71)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="1">
+        <f>AVERAGE(G53,G55,G57,G58,G59,G62,G64,G66,G69,G71)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>62</v>
       </c>
@@ -2913,8 +3310,11 @@
       <c r="F74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -2933,8 +3333,11 @@
       <c r="F75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>64</v>
       </c>
@@ -2953,8 +3356,11 @@
       <c r="F76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>65</v>
       </c>
@@ -2973,8 +3379,11 @@
       <c r="F77" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -2993,8 +3402,11 @@
       <c r="F78" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -3013,8 +3425,11 @@
       <c r="F79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -3033,8 +3448,11 @@
       <c r="F80" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>69</v>
       </c>
@@ -3053,8 +3471,11 @@
       <c r="F81" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>70</v>
       </c>
@@ -3073,8 +3494,11 @@
       <c r="F82" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>71</v>
       </c>
@@ -3093,8 +3517,11 @@
       <c r="F83" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>226</v>
       </c>
@@ -3118,8 +3545,12 @@
         <f>AVERAGE(F74:F83)</f>
         <v>2.1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="1">
+        <f>AVERAGE(G74:G83)</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>72</v>
       </c>
@@ -3129,8 +3560,20 @@
       <c r="C85" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D85" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E85" t="s">
+        <v>253</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="G85" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -3140,8 +3583,20 @@
       <c r="C86" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>75</v>
       </c>
@@ -3151,14 +3606,38 @@
       <c r="C87" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>74</v>
       </c>
       <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -3168,8 +3647,20 @@
       <c r="C89" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="1">
+        <v>5</v>
+      </c>
+      <c r="E89" s="1">
+        <v>5</v>
+      </c>
+      <c r="F89" s="1">
+        <v>5</v>
+      </c>
+      <c r="G89" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -3179,8 +3670,20 @@
       <c r="C90" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D90" s="1">
+        <v>3</v>
+      </c>
+      <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>3</v>
+      </c>
+      <c r="G90" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -3190,8 +3693,20 @@
       <c r="C91" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D91" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="F91" t="s">
+        <v>258</v>
+      </c>
+      <c r="G91" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>84</v>
       </c>
@@ -3201,8 +3716,20 @@
       <c r="C92" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>79</v>
       </c>
@@ -3210,15 +3737,39 @@
       <c r="C93" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D93" s="1">
+        <v>1</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>80</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F94" s="1">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>81</v>
       </c>
@@ -3228,8 +3779,20 @@
       <c r="C95" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="1">
+        <v>4</v>
+      </c>
+      <c r="E95" s="1">
+        <v>5</v>
+      </c>
+      <c r="F95" s="1">
+        <v>1</v>
+      </c>
+      <c r="G95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>82</v>
       </c>
@@ -3239,8 +3802,20 @@
       <c r="C96" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="1">
+        <v>3</v>
+      </c>
+      <c r="E96" s="1">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1">
+        <v>3</v>
+      </c>
+      <c r="G96" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -3250,8 +3825,20 @@
       <c r="C97" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="1">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1">
+        <v>0</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -3261,8 +3848,20 @@
       <c r="C98" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="G98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>86</v>
       </c>
@@ -3272,8 +3871,20 @@
       <c r="C99" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="1">
+        <v>1</v>
+      </c>
+      <c r="E99" s="1">
+        <v>1</v>
+      </c>
+      <c r="F99" s="1">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -3283,15 +3894,39 @@
       <c r="C100" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E100" s="1">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>88</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0</v>
+      </c>
+      <c r="F101" s="1">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -3301,8 +3936,20 @@
       <c r="C102" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="1">
+        <v>3</v>
+      </c>
+      <c r="E102" s="1">
+        <v>5</v>
+      </c>
+      <c r="F102" s="1">
+        <v>4</v>
+      </c>
+      <c r="G102" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>90</v>
       </c>
@@ -3312,8 +3959,20 @@
       <c r="C103" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="1">
+        <v>3</v>
+      </c>
+      <c r="E103" s="1">
+        <v>3</v>
+      </c>
+      <c r="F103" s="1">
+        <v>3</v>
+      </c>
+      <c r="G103" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -3323,8 +3982,20 @@
       <c r="C104" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="1">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>91</v>
       </c>
@@ -3334,8 +4005,20 @@
       <c r="C105" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>92</v>
       </c>
@@ -3345,8 +4028,20 @@
       <c r="C106" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="1">
+        <v>1</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>93</v>
       </c>
@@ -3356,16 +4051,40 @@
       <c r="C107" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="1">
+        <v>1</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F107" s="1">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>94</v>
       </c>
       <c r="C108" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="1">
+        <v>0</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0</v>
+      </c>
+      <c r="F108" s="1">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>95</v>
       </c>
@@ -3375,8 +4094,20 @@
       <c r="C109" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="1">
+        <v>3</v>
+      </c>
+      <c r="E109" s="1">
+        <v>5</v>
+      </c>
+      <c r="F109" s="1">
+        <v>3</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>96</v>
       </c>
@@ -3386,8 +4117,20 @@
       <c r="C110" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="1">
+        <v>3</v>
+      </c>
+      <c r="E110" s="1">
+        <v>3</v>
+      </c>
+      <c r="F110" s="1">
+        <v>3</v>
+      </c>
+      <c r="G110" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -3397,8 +4140,20 @@
       <c r="C111" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="1">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -3408,8 +4163,15 @@
       <c r="C112" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E112" s="1"/>
+      <c r="F112" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>98</v>
       </c>
@@ -3419,8 +4181,15 @@
       <c r="C113" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E113" s="1"/>
+      <c r="F113" s="1">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>99</v>
       </c>
@@ -3430,16 +4199,28 @@
       <c r="C114" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="1">
+        <v>1</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>100</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -3449,8 +4230,14 @@
       <c r="C116" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F116" s="1">
+        <v>3</v>
+      </c>
+      <c r="G116" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>102</v>
       </c>
@@ -3460,8 +4247,14 @@
       <c r="C117" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F117" s="1">
+        <v>2</v>
+      </c>
+      <c r="G117" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>109</v>
       </c>
@@ -3471,8 +4264,14 @@
       <c r="C118" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F118" s="1">
+        <v>0</v>
+      </c>
+      <c r="G118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>111</v>
       </c>
@@ -3482,8 +4281,20 @@
       <c r="C119" s="4" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D119" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>113</v>
       </c>
@@ -3493,8 +4304,20 @@
       <c r="C120" s="5" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D120" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="G120" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>115</v>
       </c>
@@ -3504,8 +4327,20 @@
       <c r="C121" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D121" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -3515,8 +4350,20 @@
       <c r="C122" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D122" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G122" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -3526,8 +4373,20 @@
       <c r="C123" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D123" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -3537,8 +4396,20 @@
       <c r="C124" s="5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D124" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -3548,9 +4419,20 @@
       <c r="C125" s="6">
         <v>1</v>
       </c>
-      <c r="D125" s="1"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D125" s="1">
+        <v>1</v>
+      </c>
+      <c r="E125" s="1">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1">
+        <v>1</v>
+      </c>
+      <c r="G125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -3569,8 +4451,11 @@
       <c r="F126" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -3589,8 +4474,11 @@
       <c r="F127" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -3609,8 +4497,11 @@
       <c r="F128" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -3629,8 +4520,11 @@
       <c r="F129" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -3649,8 +4543,11 @@
       <c r="F130" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -3669,8 +4566,11 @@
       <c r="F131" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>227</v>
       </c>
@@ -3694,8 +4594,12 @@
         <f>AVERAGE(F126:F131)</f>
         <v>56.666666666666664</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132" s="1">
+        <f>AVERAGE(G126:G131)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -3714,8 +4618,11 @@
       <c r="F133" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -3734,8 +4641,11 @@
       <c r="F134" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -3754,8 +4664,11 @@
       <c r="F135" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -3774,8 +4687,11 @@
       <c r="F136" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -3794,8 +4710,11 @@
       <c r="F137" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>135</v>
       </c>
@@ -3814,8 +4733,11 @@
       <c r="F138" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -3834,8 +4756,11 @@
       <c r="F139" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>137</v>
       </c>
@@ -3854,8 +4779,11 @@
       <c r="F140" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>228</v>
       </c>
@@ -3879,8 +4807,12 @@
         <f>AVERAGE(F133,F137,F139,F140)</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141" s="1">
+        <f>AVERAGE(G133,G137,G139,G140)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>229</v>
       </c>
@@ -3904,8 +4836,12 @@
         <f>AVERAGE(F134,F135,F136,F138)</f>
         <v>92.5</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142" s="1">
+        <f>AVERAGE(G134,G135,G136,G138)</f>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -3924,8 +4860,11 @@
       <c r="F143" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>139</v>
       </c>
@@ -3944,8 +4883,11 @@
       <c r="F144" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -3964,8 +4906,11 @@
       <c r="F145" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>141</v>
       </c>
@@ -3984,8 +4929,11 @@
       <c r="F146" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>142</v>
       </c>
@@ -4004,8 +4952,11 @@
       <c r="F147" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>143</v>
       </c>
@@ -4024,8 +4975,11 @@
       <c r="F148" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>230</v>
       </c>
@@ -4038,16 +4992,23 @@
         <v>81.5</v>
       </c>
       <c r="D149" s="1">
-        <v>20</v>
+        <f t="shared" ref="D149:F149" si="2">AVERAGE(D143:D148)</f>
+        <v>28.333333333333332</v>
       </c>
       <c r="E149" s="1">
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="F149" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G149" s="1">
+        <f>AVERAGE(G143:G148)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>144</v>
       </c>
@@ -4063,8 +5024,14 @@
       <c r="E150" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F150" s="1">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -4080,8 +5047,14 @@
       <c r="E151" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F151" s="1">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>146</v>
       </c>
@@ -4097,8 +5070,14 @@
       <c r="E152" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F152" s="1">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>147</v>
       </c>
@@ -4114,8 +5093,14 @@
       <c r="E153" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F153" s="1">
+        <v>0</v>
+      </c>
+      <c r="G153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>148</v>
       </c>
@@ -4131,8 +5116,14 @@
       <c r="E154" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F154" s="1">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>149</v>
       </c>
@@ -4148,8 +5139,14 @@
       <c r="E155" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F155" s="1">
+        <v>0</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>150</v>
       </c>
@@ -4165,8 +5162,14 @@
       <c r="E156" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F156" s="1">
+        <v>1</v>
+      </c>
+      <c r="G156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>151</v>
       </c>
@@ -4182,8 +5185,14 @@
       <c r="E157" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F157" s="1">
+        <v>1</v>
+      </c>
+      <c r="G157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -4199,8 +5208,14 @@
       <c r="E158" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F158" s="1">
+        <v>0</v>
+      </c>
+      <c r="G158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>153</v>
       </c>
@@ -4216,8 +5231,14 @@
       <c r="E159" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F159" s="1">
+        <v>0</v>
+      </c>
+      <c r="G159" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>154</v>
       </c>
@@ -4233,8 +5254,14 @@
       <c r="E160" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160" s="1">
+        <v>0</v>
+      </c>
+      <c r="G160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>155</v>
       </c>
@@ -4250,8 +5277,14 @@
       <c r="E161" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161" s="1">
+        <v>0</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -4267,8 +5300,14 @@
       <c r="E162" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162" s="1">
+        <v>0</v>
+      </c>
+      <c r="G162" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>156</v>
       </c>
@@ -4284,8 +5323,14 @@
       <c r="E163" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163" s="1">
+        <v>0</v>
+      </c>
+      <c r="G163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>157</v>
       </c>
@@ -4301,8 +5346,14 @@
       <c r="E164" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164" s="1">
+        <v>1</v>
+      </c>
+      <c r="G164" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>158</v>
       </c>
@@ -4318,8 +5369,14 @@
       <c r="E165" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165" s="1">
+        <v>0</v>
+      </c>
+      <c r="G165" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>159</v>
       </c>
@@ -4335,8 +5392,14 @@
       <c r="E166" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166" s="1">
+        <v>0</v>
+      </c>
+      <c r="G166" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>161</v>
       </c>
@@ -4352,8 +5415,14 @@
       <c r="E167" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167" s="1">
+        <v>0</v>
+      </c>
+      <c r="G167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>162</v>
       </c>
@@ -4369,8 +5438,14 @@
       <c r="E168" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168" s="1">
+        <v>0</v>
+      </c>
+      <c r="G168" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>206</v>
       </c>
@@ -4386,8 +5461,14 @@
       <c r="E169" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169" s="1">
+        <v>0</v>
+      </c>
+      <c r="G169" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>163</v>
       </c>
@@ -4403,8 +5484,14 @@
       <c r="E170" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170" s="1">
+        <v>0</v>
+      </c>
+      <c r="G170" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>164</v>
       </c>
@@ -4420,8 +5507,14 @@
       <c r="E171" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171" s="1">
+        <v>0</v>
+      </c>
+      <c r="G171" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>165</v>
       </c>
@@ -4437,8 +5530,14 @@
       <c r="E172" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172" s="1">
+        <v>0</v>
+      </c>
+      <c r="G172" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>166</v>
       </c>
@@ -4454,8 +5553,14 @@
       <c r="E173" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173" s="1">
+        <v>2</v>
+      </c>
+      <c r="G173" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>167</v>
       </c>
@@ -4471,8 +5576,14 @@
       <c r="E174" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174" s="1">
+        <v>0</v>
+      </c>
+      <c r="G174" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>231</v>
       </c>
@@ -4492,8 +5603,16 @@
         <f>AVERAGE(E150:E174)</f>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175" s="1">
+        <f>AVERAGE(F150:F174)</f>
+        <v>0.2</v>
+      </c>
+      <c r="G175" s="1">
+        <f>AVERAGE(G150:G174)</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>168</v>
       </c>
@@ -4509,8 +5628,14 @@
       <c r="E176" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176" s="1">
+        <v>5</v>
+      </c>
+      <c r="G176" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>169</v>
       </c>
@@ -4526,8 +5651,14 @@
       <c r="E177" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177" s="1">
+        <v>5</v>
+      </c>
+      <c r="G177" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>170</v>
       </c>
@@ -4543,8 +5674,14 @@
       <c r="E178" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178" s="1">
+        <v>5</v>
+      </c>
+      <c r="G178" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>171</v>
       </c>
@@ -4560,8 +5697,14 @@
       <c r="E179" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179" s="1">
+        <v>5</v>
+      </c>
+      <c r="G179" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>172</v>
       </c>
@@ -4577,8 +5720,14 @@
       <c r="E180" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180" s="1">
+        <v>5</v>
+      </c>
+      <c r="G180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>173</v>
       </c>
@@ -4594,8 +5743,14 @@
       <c r="E181" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F181" s="1">
+        <v>3</v>
+      </c>
+      <c r="G181" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>174</v>
       </c>
@@ -4611,8 +5766,14 @@
       <c r="E182" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F182" s="1">
+        <v>5</v>
+      </c>
+      <c r="G182" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>175</v>
       </c>
@@ -4628,8 +5789,14 @@
       <c r="E183" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F183" s="1">
+        <v>4</v>
+      </c>
+      <c r="G183" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>176</v>
       </c>
@@ -4645,8 +5812,14 @@
       <c r="E184" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F184" s="1">
+        <v>4</v>
+      </c>
+      <c r="G184" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>177</v>
       </c>
@@ -4662,8 +5835,14 @@
       <c r="E185" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F185" s="1">
+        <v>5</v>
+      </c>
+      <c r="G185" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>178</v>
       </c>
@@ -4679,8 +5858,14 @@
       <c r="E186" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F186" s="1">
+        <v>5</v>
+      </c>
+      <c r="G186" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>197</v>
       </c>
@@ -4696,8 +5881,14 @@
       <c r="E187" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F187" s="1">
+        <v>4</v>
+      </c>
+      <c r="G187" s="9">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>179</v>
       </c>
@@ -4713,8 +5904,14 @@
       <c r="E188" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F188" s="1">
+        <v>5</v>
+      </c>
+      <c r="G188" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>180</v>
       </c>
@@ -4730,8 +5927,14 @@
       <c r="E189" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F189" s="1">
+        <v>5</v>
+      </c>
+      <c r="G189" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>181</v>
       </c>
@@ -4747,8 +5950,14 @@
       <c r="E190" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F190" s="1">
+        <v>5</v>
+      </c>
+      <c r="G190" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>182</v>
       </c>
@@ -4764,8 +5973,14 @@
       <c r="E191" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F191" s="1">
+        <v>5</v>
+      </c>
+      <c r="G191" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>183</v>
       </c>
@@ -4781,8 +5996,14 @@
       <c r="E192" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F192" s="1">
+        <v>3</v>
+      </c>
+      <c r="G192" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>184</v>
       </c>
@@ -4798,8 +6019,14 @@
       <c r="E193" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F193" s="1">
+        <v>4</v>
+      </c>
+      <c r="G193" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>185</v>
       </c>
@@ -4815,8 +6042,14 @@
       <c r="E194" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F194" s="1">
+        <v>5</v>
+      </c>
+      <c r="G194" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>186</v>
       </c>
@@ -4832,8 +6065,14 @@
       <c r="E195" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F195" s="1">
+        <v>5</v>
+      </c>
+      <c r="G195" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>187</v>
       </c>
@@ -4849,8 +6088,14 @@
       <c r="E196" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F196" s="1">
+        <v>5</v>
+      </c>
+      <c r="G196" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>188</v>
       </c>
@@ -4866,8 +6111,14 @@
       <c r="E197" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F197" s="1">
+        <v>5</v>
+      </c>
+      <c r="G197" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>189</v>
       </c>
@@ -4883,8 +6134,14 @@
       <c r="E198" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F198" s="1">
+        <v>4</v>
+      </c>
+      <c r="G198" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>190</v>
       </c>
@@ -4900,8 +6157,14 @@
       <c r="E199" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F199" s="1">
+        <v>5</v>
+      </c>
+      <c r="G199" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>191</v>
       </c>
@@ -4917,8 +6180,14 @@
       <c r="E200" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F200" s="1">
+        <v>5</v>
+      </c>
+      <c r="G200" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>192</v>
       </c>
@@ -4934,8 +6203,14 @@
       <c r="E201" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F201" s="1">
+        <v>5</v>
+      </c>
+      <c r="G201" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>193</v>
       </c>
@@ -4951,8 +6226,14 @@
       <c r="E202" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F202" s="1">
+        <v>5</v>
+      </c>
+      <c r="G202" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>194</v>
       </c>
@@ -4968,8 +6249,14 @@
       <c r="E203" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F203" s="1">
+        <v>4</v>
+      </c>
+      <c r="G203" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>195</v>
       </c>
@@ -4985,8 +6272,14 @@
       <c r="E204" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F204" s="1">
+        <v>5</v>
+      </c>
+      <c r="G204" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>196</v>
       </c>
@@ -5002,8 +6295,14 @@
       <c r="E205" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F205" s="1">
+        <v>4</v>
+      </c>
+      <c r="G205" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>232</v>
       </c>
@@ -5023,12 +6322,20 @@
         <f>AVERAGE(E176:E205)</f>
         <v>3.2</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F206" s="1">
+        <f>AVERAGE(F176:F205)</f>
+        <v>4.6333333333333337</v>
+      </c>
+      <c r="G206" s="1">
+        <f>AVERAGE(G176:G205)</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
     </row>

</xml_diff>

<commit_message>
Just added these to work on from home
</commit_message>
<xml_diff>
--- a/DataCollection/QuestionnaireData/QuestionnaireScores.xlsx
+++ b/DataCollection/QuestionnaireData/QuestionnaireScores.xlsx
@@ -909,7 +909,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -990,7 +990,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1314,7 +1314,7 @@
   <dimension ref="A1:AL209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,6 +1513,14 @@
       <c r="H4" s="1">
         <v>23</v>
       </c>
+      <c r="I4">
+        <f>AVERAGE(B4:G4)</f>
+        <v>26.5</v>
+      </c>
+      <c r="J4">
+        <f>_xlfn.STDEV.P(B4:G4)</f>
+        <v>2.9860788111948193</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="W4" s="1"/>
@@ -1949,27 +1957,27 @@
         <v>235</v>
       </c>
       <c r="B21" s="1">
-        <f>AVERAGE(B16:B20)</f>
+        <f t="shared" ref="B21:G21" si="0">AVERAGE(B16:B20)</f>
         <v>1.2</v>
       </c>
       <c r="C21" s="1">
-        <f>AVERAGE(C16:C20)</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="D21" s="1">
-        <f>AVERAGE(D16:D20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <f>AVERAGE(E16:E20)</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="F21" s="1">
-        <f>AVERAGE(F16:F20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G21" s="1">
-        <f>AVERAGE(G16:G20)</f>
+        <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
       <c r="P21" s="1"/>
@@ -2114,15 +2122,15 @@
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E27:G27" si="0">AVERAGE(E16:E26)</f>
+        <f t="shared" ref="E27:G27" si="1">AVERAGE(E16:E26)</f>
         <v>1.3818181818181818</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8909090909090909</v>
       </c>
       <c r="H27" s="1"/>
@@ -2206,27 +2214,27 @@
         <v>221</v>
       </c>
       <c r="B31" s="1">
-        <f>AVERAGE(B28:B30)</f>
+        <f t="shared" ref="B31:G31" si="2">AVERAGE(B28:B30)</f>
         <v>81</v>
       </c>
       <c r="C31" s="1">
-        <f>AVERAGE(C28:C30)</f>
+        <f t="shared" si="2"/>
         <v>89.333333333333329</v>
       </c>
       <c r="D31">
-        <f>AVERAGE(D28:D30)</f>
+        <f t="shared" si="2"/>
         <v>93.333333333333329</v>
       </c>
       <c r="E31" s="1">
-        <f>AVERAGE(E28:E30)</f>
+        <f t="shared" si="2"/>
         <v>56.5</v>
       </c>
       <c r="F31" s="1">
-        <f>AVERAGE(F28:F30)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G31" s="1">
-        <f>AVERAGE(G28:G30)</f>
+        <f t="shared" si="2"/>
         <v>61.666666666666664</v>
       </c>
     </row>
@@ -2749,27 +2757,27 @@
         <v>223</v>
       </c>
       <c r="B51" s="1">
-        <f>AVERAGE(B42:B50)</f>
+        <f t="shared" ref="B51:G51" si="3">AVERAGE(B42:B50)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="C51" s="1">
-        <f>AVERAGE(C42:C50)</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="D51">
-        <f>AVERAGE(D42:D50)</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E51">
-        <f>AVERAGE(E42:E50)</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F51">
-        <f>AVERAGE(F42:F50)</f>
+        <f t="shared" si="3"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="G51">
-        <f>AVERAGE(G42:G50)</f>
+        <f t="shared" si="3"/>
         <v>2.3333333333333335</v>
       </c>
     </row>
@@ -3238,11 +3246,11 @@
         <v>224</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" ref="B72:C72" si="1">AVERAGE(B52,B54,B56,B60,B61,B63,B65,B67,B68,B70)</f>
+        <f t="shared" ref="B72:C72" si="4">AVERAGE(B52,B54,B56,B60,B61,B63,B65,B67,B68,B70)</f>
         <v>2.4</v>
       </c>
       <c r="C72" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.7</v>
       </c>
       <c r="D72" s="1">
@@ -3267,27 +3275,27 @@
         <v>225</v>
       </c>
       <c r="B73" s="1">
-        <f>AVERAGE(B53,B55,B57,B58,B59,B62,B64,B66,B69,B71)</f>
+        <f t="shared" ref="B73:G73" si="5">AVERAGE(B53,B55,B57,B58,B59,B62,B64,B66,B69,B71)</f>
         <v>0.5</v>
       </c>
       <c r="C73" s="1">
-        <f>AVERAGE(C53,C55,C57,C58,C59,C62,C64,C66,C69,C71)</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="D73" s="1">
-        <f>AVERAGE(D53,D55,D57,D58,D59,D62,D64,D66,D69,D71)</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="E73" s="1">
-        <f>AVERAGE(E53,E55,E57,E58,E59,E62,E64,E66,E69,E71)</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="F73" s="1">
-        <f>AVERAGE(F53,F55,F57,F58,F59,F62,F64,F66,F69,F71)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G73" s="1">
-        <f>AVERAGE(G53,G55,G57,G58,G59,G62,G64,G66,G69,G71)</f>
+        <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
     </row>
@@ -3526,27 +3534,27 @@
         <v>226</v>
       </c>
       <c r="B84" s="1">
-        <f>AVERAGE(B74:B83)</f>
+        <f t="shared" ref="B84:G84" si="6">AVERAGE(B74:B83)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="C84" s="1">
-        <f>AVERAGE(C74:C83)</f>
+        <f t="shared" si="6"/>
         <v>2.6</v>
       </c>
       <c r="D84" s="1">
-        <f>AVERAGE(D74:D83)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="E84" s="1">
-        <f>AVERAGE(E74:E83)</f>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F84" s="1">
-        <f>AVERAGE(F74:F83)</f>
+        <f t="shared" si="6"/>
         <v>2.1</v>
       </c>
       <c r="G84" s="1">
-        <f>AVERAGE(G74:G83)</f>
+        <f t="shared" si="6"/>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -4575,27 +4583,27 @@
         <v>227</v>
       </c>
       <c r="B132" s="1">
-        <f>AVERAGE(B126:B131)</f>
+        <f t="shared" ref="B132:G132" si="7">AVERAGE(B126:B131)</f>
         <v>40</v>
       </c>
       <c r="C132" s="1">
-        <f>AVERAGE(C126:C131)</f>
+        <f t="shared" si="7"/>
         <v>79.166666666666671</v>
       </c>
       <c r="D132" s="1">
-        <f>AVERAGE(D126:D131)</f>
+        <f t="shared" si="7"/>
         <v>64.166666666666671</v>
       </c>
       <c r="E132" s="1">
-        <f>AVERAGE(E126:E131)</f>
+        <f t="shared" si="7"/>
         <v>17.666666666666668</v>
       </c>
       <c r="F132" s="1">
-        <f>AVERAGE(F126:F131)</f>
+        <f t="shared" si="7"/>
         <v>56.666666666666664</v>
       </c>
       <c r="G132" s="1">
-        <f>AVERAGE(G126:G131)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4788,27 +4796,27 @@
         <v>228</v>
       </c>
       <c r="B141" s="1">
-        <f>AVERAGE(B133,B137,B139,B140)</f>
+        <f t="shared" ref="B141:G141" si="8">AVERAGE(B133,B137,B139,B140)</f>
         <v>82.5</v>
       </c>
       <c r="C141" s="1">
-        <f>AVERAGE(C133,C137,C139,C140)</f>
+        <f t="shared" si="8"/>
         <v>93.75</v>
       </c>
       <c r="D141" s="1">
-        <f>AVERAGE(D133,D137,D139,D140)</f>
+        <f t="shared" si="8"/>
         <v>86.25</v>
       </c>
       <c r="E141" s="1">
-        <f>AVERAGE(E133,E137,E139,E140)</f>
+        <f t="shared" si="8"/>
         <v>66.25</v>
       </c>
       <c r="F141" s="1">
-        <f>AVERAGE(F133,F137,F139,F140)</f>
+        <f t="shared" si="8"/>
         <v>85</v>
       </c>
       <c r="G141" s="1">
-        <f>AVERAGE(G133,G137,G139,G140)</f>
+        <f t="shared" si="8"/>
         <v>1.25</v>
       </c>
     </row>
@@ -4817,27 +4825,27 @@
         <v>229</v>
       </c>
       <c r="B142" s="1">
-        <f>AVERAGE(B134,B135,B136,B138)</f>
+        <f t="shared" ref="B142:G142" si="9">AVERAGE(B134,B135,B136,B138)</f>
         <v>65</v>
       </c>
       <c r="C142" s="1">
-        <f>AVERAGE(C134,C135,C136,C138)</f>
+        <f t="shared" si="9"/>
         <v>92.25</v>
       </c>
       <c r="D142" s="1">
-        <f>AVERAGE(D134,D135,D136,D138)</f>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="E142" s="1">
-        <f>AVERAGE(E134,E135,E136,E138)</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="F142" s="1">
-        <f>AVERAGE(F134,F135,F136,F138)</f>
+        <f t="shared" si="9"/>
         <v>92.5</v>
       </c>
       <c r="G142" s="1">
-        <f>AVERAGE(G134,G135,G136,G138)</f>
+        <f t="shared" si="9"/>
         <v>11.25</v>
       </c>
     </row>
@@ -4992,15 +5000,15 @@
         <v>81.5</v>
       </c>
       <c r="D149" s="1">
-        <f t="shared" ref="D149:F149" si="2">AVERAGE(D143:D148)</f>
+        <f t="shared" ref="D149:F149" si="10">AVERAGE(D143:D148)</f>
         <v>28.333333333333332</v>
       </c>
       <c r="E149" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F149" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
       <c r="G149" s="1">
@@ -5588,27 +5596,27 @@
         <v>231</v>
       </c>
       <c r="B175" s="1">
-        <f>AVERAGE(B150:B174)</f>
+        <f t="shared" ref="B175:G175" si="11">AVERAGE(B150:B174)</f>
         <v>0.76</v>
       </c>
       <c r="C175" s="1">
-        <f>AVERAGE(C150:C174)</f>
+        <f t="shared" si="11"/>
         <v>3.2</v>
       </c>
       <c r="D175" s="1">
-        <f>AVERAGE(D150:D174)</f>
+        <f t="shared" si="11"/>
         <v>0.88</v>
       </c>
       <c r="E175" s="1">
-        <f>AVERAGE(E150:E174)</f>
+        <f t="shared" si="11"/>
         <v>1.6</v>
       </c>
       <c r="F175" s="1">
-        <f>AVERAGE(F150:F174)</f>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="G175" s="1">
-        <f>AVERAGE(G150:G174)</f>
+        <f t="shared" si="11"/>
         <v>0.22</v>
       </c>
     </row>
@@ -6307,27 +6315,27 @@
         <v>232</v>
       </c>
       <c r="B206" s="1">
-        <f>AVERAGE(B176:B205)</f>
+        <f t="shared" ref="B206:G206" si="12">AVERAGE(B176:B205)</f>
         <v>3.3666666666666667</v>
       </c>
       <c r="C206" s="1">
-        <f>AVERAGE(C176:C205)</f>
+        <f t="shared" si="12"/>
         <v>4.4833333333333334</v>
       </c>
       <c r="D206" s="1">
-        <f>AVERAGE(D176:D205)</f>
+        <f t="shared" si="12"/>
         <v>3.7333333333333334</v>
       </c>
       <c r="E206" s="1">
-        <f>AVERAGE(E176:E205)</f>
+        <f t="shared" si="12"/>
         <v>3.2</v>
       </c>
       <c r="F206" s="1">
-        <f>AVERAGE(F176:F205)</f>
+        <f t="shared" si="12"/>
         <v>4.6333333333333337</v>
       </c>
       <c r="G206" s="1">
-        <f>AVERAGE(G176:G205)</f>
+        <f t="shared" si="12"/>
         <v>1.75</v>
       </c>
     </row>

</xml_diff>